<commit_message>
Added Func to Select and Recombine
</commit_message>
<xml_diff>
--- a/GA.xlsx
+++ b/GA.xlsx
@@ -14,66 +14,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>100000111000111011</t>
-  </si>
-  <si>
-    <t>000000001011100011</t>
-  </si>
-  <si>
-    <t>100010000000100010</t>
-  </si>
-  <si>
-    <t>010010000110110111</t>
-  </si>
-  <si>
-    <t>001100011010101111</t>
-  </si>
-  <si>
-    <t>111111111000101111</t>
-  </si>
-  <si>
-    <t>001010010011111011</t>
-  </si>
-  <si>
-    <t>001011111110101100</t>
-  </si>
-  <si>
-    <t>001111010011000101</t>
-  </si>
-  <si>
-    <t>001001100101100010</t>
-  </si>
-  <si>
-    <t>000000110111000010</t>
-  </si>
-  <si>
-    <t>011100000001110110</t>
-  </si>
-  <si>
-    <t>001001010000011000</t>
-  </si>
-  <si>
-    <t>001001111011110000</t>
-  </si>
-  <si>
-    <t>010110010110010010</t>
-  </si>
-  <si>
-    <t>100110101101010111</t>
-  </si>
-  <si>
-    <t>000101110010010000</t>
-  </si>
-  <si>
-    <t>111000110110111010</t>
-  </si>
-  <si>
-    <t>001100110100110100</t>
-  </si>
-  <si>
-    <t>101010010101010111</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+  <si>
+    <t>011000111010101011</t>
+  </si>
+  <si>
+    <t>100110111110001000</t>
+  </si>
+  <si>
+    <t>001011011011100100</t>
+  </si>
+  <si>
+    <t>101001100111001101</t>
+  </si>
+  <si>
+    <t>011111111111100001</t>
+  </si>
+  <si>
+    <t>000011100001000111</t>
+  </si>
+  <si>
+    <t>010010011101001100</t>
+  </si>
+  <si>
+    <t>111100110100011001</t>
+  </si>
+  <si>
+    <t>101010000000001001</t>
+  </si>
+  <si>
+    <t>000110000000010110</t>
+  </si>
+  <si>
+    <t>110101100011111100</t>
+  </si>
+  <si>
+    <t>101010010010111000</t>
+  </si>
+  <si>
+    <t>001101000001101000</t>
+  </si>
+  <si>
+    <t>100010001100000110</t>
+  </si>
+  <si>
+    <t>001110111111001000</t>
+  </si>
+  <si>
+    <t>000100100011110000</t>
+  </si>
+  <si>
+    <t>010101010111011111</t>
+  </si>
+  <si>
+    <t>001001101110111100</t>
+  </si>
+  <si>
+    <t>001011000111100011</t>
+  </si>
+  <si>
+    <t>110010001101111010</t>
   </si>
 </sst>
 </file>
@@ -405,464 +405,530 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1">
-        <v>134715</v>
+        <v>102059</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1">
-        <v>13.33357366017784</v>
+        <v>10.34381616140809</v>
       </c>
       <c r="D1">
-        <v>2.776976746053079</v>
+        <v>21.68004793876453</v>
       </c>
       <c r="E1">
-        <v>0.001808424249414455</v>
+        <v>0.01866106677401547</v>
       </c>
       <c r="F1">
-        <v>0.002</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>0.019</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
-        <v>739</v>
+        <v>159624</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1.067657728796878</v>
+        <v>15.61406942012566</v>
       </c>
       <c r="D2">
-        <v>194.1101611619534</v>
+        <v>0.3770812527334592</v>
       </c>
       <c r="E2">
-        <v>0.1264085207058176</v>
+        <v>0.000324572088418061</v>
       </c>
       <c r="F2">
-        <v>0.128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>0.019</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
-        <v>139298</v>
+        <v>46820</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>13.75316144241883</v>
+        <v>5.286515375195981</v>
       </c>
       <c r="D3">
-        <v>1.554606388671086</v>
+        <v>94.35178355630408</v>
       </c>
       <c r="E3">
-        <v>0.001012391585764359</v>
+        <v>0.08121314759841723</v>
       </c>
       <c r="F3">
-        <v>0.129</v>
+        <v>0.1</v>
       </c>
       <c r="G3">
-        <v>0.386</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>0.731</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
-        <v>74167</v>
+        <v>170445</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>7.790217553014957</v>
+        <v>16.60476533800254</v>
       </c>
       <c r="D4">
-        <v>51.98096293285364</v>
+        <v>2.575271790054407</v>
       </c>
       <c r="E4">
-        <v>0.03385106987636607</v>
+        <v>0.002216661096469063</v>
       </c>
       <c r="F4">
-        <v>0.163</v>
+        <v>0.102</v>
       </c>
       <c r="G4">
-        <v>0.515</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>0.858</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
-        <v>50863</v>
+        <v>131041</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>5.65666449228093</v>
+        <v>12.99720763094952</v>
       </c>
       <c r="D5">
-        <v>87.29791840980397</v>
+        <v>4.011177273526835</v>
       </c>
       <c r="E5">
-        <v>0.05685019609907694</v>
+        <v>0.003452614457086074</v>
       </c>
       <c r="F5">
-        <v>0.22</v>
+        <v>0.106</v>
       </c>
       <c r="G5">
-        <v>0.199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>0.223</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
-        <v>261679</v>
+        <v>14407</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>24.95751936919925</v>
+        <v>2.319005275746444</v>
       </c>
       <c r="D6">
-        <v>99.15219198797831</v>
+        <v>160.8076271965465</v>
       </c>
       <c r="E6">
-        <v>0.06456994234053638</v>
+        <v>0.1384149092917895</v>
       </c>
       <c r="F6">
-        <v>0.285</v>
+        <v>0.244</v>
       </c>
       <c r="G6">
-        <v>0.523</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>0.412</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
-        <v>42235</v>
+        <v>75596</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7">
-        <v>4.866744486787745</v>
+        <v>7.921046909511221</v>
       </c>
       <c r="D7">
-        <v>102.6828672960466</v>
+        <v>50.11157685734064</v>
       </c>
       <c r="E7">
-        <v>0.06686919056182396</v>
+        <v>0.04313346006094358</v>
       </c>
       <c r="F7">
-        <v>0.351</v>
+        <v>0.287</v>
       </c>
       <c r="G7">
-        <v>0.869</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>0.092</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
-        <v>49068</v>
+        <v>249113</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>5.492326707178906</v>
+        <v>23.80706332040146</v>
       </c>
       <c r="D8">
-        <v>90.3958514430235</v>
+        <v>77.56436432956075</v>
       </c>
       <c r="E8">
-        <v>0.05886763366973681</v>
+        <v>0.06676340320493224</v>
       </c>
       <c r="F8">
-        <v>0.41</v>
+        <v>0.354</v>
       </c>
       <c r="G8">
-        <v>0.6850000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>0.768</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
-        <v>62661</v>
+        <v>172041</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9">
-        <v>6.7368077728568</v>
+        <v>16.75088405946373</v>
       </c>
       <c r="D9">
-        <v>68.28034578271981</v>
+        <v>3.065594989684187</v>
       </c>
       <c r="E9">
-        <v>0.04446556250331466</v>
+        <v>0.002638706010529417</v>
       </c>
       <c r="F9">
-        <v>0.455</v>
+        <v>0.357</v>
       </c>
       <c r="G9">
-        <v>0.954</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>0.914</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
-        <v>39266</v>
+        <v>24598</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10">
-        <v>4.594923381513143</v>
+        <v>3.25202275094128</v>
       </c>
       <c r="D10">
-        <v>108.2656194365819</v>
+        <v>138.0149694444013</v>
       </c>
       <c r="E10">
-        <v>0.07050479333154967</v>
+        <v>0.11879616539088</v>
       </c>
       <c r="F10">
-        <v>0.525</v>
+        <v>0.476</v>
       </c>
       <c r="G10">
-        <v>0.751</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>0.626</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
-        <v>3522</v>
+        <v>219388</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>1.322449960517733</v>
+        <v>21.08564790972866</v>
       </c>
       <c r="D11">
-        <v>187.0753750825413</v>
+        <v>37.03511048118477</v>
       </c>
       <c r="E11">
-        <v>0.1218273236347461</v>
+        <v>0.03187791243010569</v>
       </c>
       <c r="F11">
+        <v>0.507</v>
+      </c>
+      <c r="G11">
         <v>0.647</v>
       </c>
-      <c r="G11">
-        <v>0.796</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
-        <v>114806</v>
+        <v>173240</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12">
-        <v>11.51084331834151</v>
+        <v>16.86065620672686</v>
       </c>
       <c r="D12">
-        <v>12.17421434916205</v>
+        <v>3.462041519631195</v>
       </c>
       <c r="E12">
-        <v>0.007928098237727652</v>
+        <v>0.002979946730502171</v>
       </c>
       <c r="F12">
-        <v>0.655</v>
+        <v>0.51</v>
       </c>
       <c r="G12">
-        <v>0.694</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>0.9330000000000001</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
-        <v>37912</v>
+        <v>53352</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13">
-        <v>4.470960506288552</v>
+        <v>5.884540117416829</v>
       </c>
       <c r="D13">
-        <v>110.8606726601354</v>
+        <v>83.09160887098319</v>
       </c>
       <c r="E13">
-        <v>0.07219474524946383</v>
+        <v>0.0715209701510538</v>
       </c>
       <c r="F13">
-        <v>0.727</v>
+        <v>0.582</v>
       </c>
       <c r="G13">
-        <v>0.006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>0.822</v>
+      </c>
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
-        <v>40688</v>
+        <v>140038</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14">
-        <v>4.725111866424051</v>
+        <v>13.82091072429933</v>
       </c>
       <c r="D14">
-        <v>105.5733261574998</v>
+        <v>1.390251520072328</v>
       </c>
       <c r="E14">
-        <v>0.06875151669380054</v>
+        <v>0.001196656784248082</v>
       </c>
       <c r="F14">
-        <v>0.796</v>
+        <v>0.583</v>
       </c>
       <c r="G14">
-        <v>0.351</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>0.63</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
-        <v>91538</v>
+        <v>61384</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15">
-        <v>9.380586168617892</v>
+        <v>6.619894485071125</v>
       </c>
       <c r="D15">
-        <v>31.57781180832854</v>
+        <v>70.22616844134134</v>
       </c>
       <c r="E15">
-        <v>0.02056411912659781</v>
+        <v>0.0604470627679714</v>
       </c>
       <c r="F15">
-        <v>0.8159999999999999</v>
+        <v>0.644</v>
       </c>
       <c r="G15">
-        <v>0.525</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>0.725</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
-        <v>158551</v>
+        <v>18672</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16">
-        <v>15.51583296139893</v>
+        <v>2.709479177395544</v>
       </c>
       <c r="D16">
-        <v>0.2660836440655899</v>
+        <v>151.0569020908737</v>
       </c>
       <c r="E16">
-        <v>0.0001732791298971792</v>
+        <v>0.1300219881688301</v>
       </c>
       <c r="F16">
-        <v>0.8169999999999999</v>
+        <v>0.774</v>
       </c>
       <c r="G16">
-        <v>0.8090000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>0.921</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
-        <v>23696</v>
+        <v>87519</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17">
-        <v>3.169441869513967</v>
+        <v>9.012634325539876</v>
       </c>
       <c r="D17">
-        <v>139.9621056788092</v>
+        <v>35.84854771970333</v>
       </c>
       <c r="E17">
-        <v>0.09114619568507874</v>
+        <v>0.03085658042078048</v>
       </c>
       <c r="F17">
-        <v>0.908</v>
+        <v>0.805</v>
       </c>
       <c r="G17">
-        <v>0.637</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>0.982</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
-        <v>232890</v>
+        <v>39868</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18">
-        <v>22.32179764479692</v>
+        <v>4.650038337853767</v>
       </c>
       <c r="D18">
-        <v>53.60872075135378</v>
+        <v>107.1217064078968</v>
       </c>
       <c r="E18">
-        <v>0.03491109917453485</v>
+        <v>0.09220483837814611</v>
       </c>
       <c r="F18">
-        <v>0.9429999999999999</v>
+        <v>0.897</v>
       </c>
       <c r="G18">
-        <v>0.186</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>0.195</v>
+      </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19">
-        <v>52532</v>
+        <v>45539</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="C19">
-        <v>5.809466588846545</v>
+        <v>5.169235875075817</v>
       </c>
       <c r="D19">
-        <v>84.46590438152795</v>
+        <v>96.64392327989634</v>
       </c>
       <c r="E19">
-        <v>0.05500593044193903</v>
+        <v>0.08318610321909405</v>
       </c>
       <c r="F19">
-        <v>0.998</v>
+        <v>0.98</v>
       </c>
       <c r="G19">
-        <v>0.803</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>0.834</v>
+      </c>
+      <c r="H19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
-        <v>173399</v>
+        <v>205690</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
       <c r="C20">
-        <v>16.87521314702281</v>
+        <v>19.83155377027042</v>
       </c>
       <c r="D20">
-        <v>3.516424346767173</v>
+        <v>23.34391183501436</v>
       </c>
       <c r="E20">
-        <v>0.002289967702813307</v>
+        <v>0.02009323497578748</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>0.914</v>
+        <v>0.418</v>
+      </c>
+      <c r="H20" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added aditional input to choose if want excel parse
</commit_message>
<xml_diff>
--- a/GA.xlsx
+++ b/GA.xlsx
@@ -14,66 +14,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
-  <si>
-    <t>011000111010101011</t>
-  </si>
-  <si>
-    <t>100110111110001000</t>
-  </si>
-  <si>
-    <t>001011011011100100</t>
-  </si>
-  <si>
-    <t>101001100111001101</t>
-  </si>
-  <si>
-    <t>011111111111100001</t>
-  </si>
-  <si>
-    <t>000011100001000111</t>
-  </si>
-  <si>
-    <t>010010011101001100</t>
-  </si>
-  <si>
-    <t>111100110100011001</t>
-  </si>
-  <si>
-    <t>101010000000001001</t>
-  </si>
-  <si>
-    <t>000110000000010110</t>
-  </si>
-  <si>
-    <t>110101100011111100</t>
-  </si>
-  <si>
-    <t>101010010010111000</t>
-  </si>
-  <si>
-    <t>001101000001101000</t>
-  </si>
-  <si>
-    <t>100010001100000110</t>
-  </si>
-  <si>
-    <t>001110111111001000</t>
-  </si>
-  <si>
-    <t>000100100011110000</t>
-  </si>
-  <si>
-    <t>010101010111011111</t>
-  </si>
-  <si>
-    <t>001001101110111100</t>
-  </si>
-  <si>
-    <t>001011000111100011</t>
-  </si>
-  <si>
-    <t>110010001101111010</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+  <si>
+    <t>101111101100101001</t>
+  </si>
+  <si>
+    <t>100000100010101001</t>
+  </si>
+  <si>
+    <t>000000101101111101</t>
+  </si>
+  <si>
+    <t>111001000110010110</t>
+  </si>
+  <si>
+    <t>011110010111000011</t>
+  </si>
+  <si>
+    <t>001100001101100101</t>
+  </si>
+  <si>
+    <t>011111000111010001</t>
+  </si>
+  <si>
+    <t>100101101010111101</t>
+  </si>
+  <si>
+    <t>111110011111110100</t>
+  </si>
+  <si>
+    <t>001001101110101100</t>
+  </si>
+  <si>
+    <t>101111011101101001</t>
+  </si>
+  <si>
+    <t>100100011100010110</t>
+  </si>
+  <si>
+    <t>010101000000111110</t>
+  </si>
+  <si>
+    <t>110001001001001111</t>
+  </si>
+  <si>
+    <t>110100100000100110</t>
+  </si>
+  <si>
+    <t>001010100100101001</t>
+  </si>
+  <si>
+    <t>100000011010110111</t>
+  </si>
+  <si>
+    <t>011000110101101100</t>
+  </si>
+  <si>
+    <t>001111110101110110</t>
+  </si>
+  <si>
+    <t>011110010000011011</t>
+  </si>
+  <si>
+    <t>000111101100101001</t>
+  </si>
+  <si>
+    <t>101000101101111101</t>
+  </si>
+  <si>
+    <t>000110011111110100</t>
+  </si>
+  <si>
+    <t>111000101101111101</t>
+  </si>
+  <si>
+    <t>000100100000100110</t>
+  </si>
+  <si>
+    <t>110000101101111101</t>
+  </si>
+  <si>
+    <t>111001101110101100</t>
+  </si>
+  <si>
+    <t>001001000110010110</t>
+  </si>
+  <si>
+    <t>001100100000100110</t>
+  </si>
+  <si>
+    <t>110010100100101001</t>
+  </si>
+  <si>
+    <t>001000110101101100</t>
+  </si>
+  <si>
+    <t>011100001101100101</t>
   </si>
 </sst>
 </file>
@@ -405,530 +441,590 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1">
-        <v>102059</v>
+        <v>195369</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1">
-        <v>10.34381616140809</v>
+        <v>18.88663439420469</v>
       </c>
       <c r="D1">
-        <v>21.68004793876453</v>
+        <v>15.10592691421484</v>
       </c>
       <c r="E1">
-        <v>0.01866106677401547</v>
+        <v>0.01754272438464307</v>
       </c>
       <c r="F1">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="G1">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
-        <v>159624</v>
+        <v>133289</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>15.61406942012566</v>
+        <v>13.20301896293245</v>
       </c>
       <c r="D2">
-        <v>0.3770812527334592</v>
+        <v>3.229140847580386</v>
       </c>
       <c r="E2">
-        <v>0.000324572088418061</v>
+        <v>0.003750046469176885</v>
       </c>
       <c r="F2">
-        <v>0.019</v>
+        <v>0.021</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
-        <v>46820</v>
+        <v>2941</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>5.286515375195981</v>
+        <v>1.269257618933178</v>
       </c>
       <c r="D3">
-        <v>94.35178355630408</v>
+        <v>188.5332863352246</v>
       </c>
       <c r="E3">
-        <v>0.08121314759841723</v>
+        <v>0.2189463445899207</v>
       </c>
       <c r="F3">
-        <v>0.1</v>
+        <v>0.24</v>
       </c>
       <c r="G3">
-        <v>0.731</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
-        <v>170445</v>
+        <v>233878</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>16.60476533800254</v>
+        <v>22.41225209141575</v>
       </c>
       <c r="D4">
-        <v>2.575271790054407</v>
+        <v>54.94148106669719</v>
       </c>
       <c r="E4">
-        <v>0.002216661096469063</v>
+        <v>0.06380431105688633</v>
       </c>
       <c r="F4">
-        <v>0.102</v>
+        <v>0.304</v>
       </c>
       <c r="G4">
-        <v>0.858</v>
+        <v>0.015</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
-        <v>131041</v>
+        <v>124355</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>12.99720763094952</v>
+        <v>12.38508371385084</v>
       </c>
       <c r="D5">
-        <v>4.011177273526835</v>
+        <v>6.837787183568136</v>
       </c>
       <c r="E5">
-        <v>0.003452614457086074</v>
+        <v>0.007940817974519869</v>
       </c>
       <c r="F5">
-        <v>0.106</v>
+        <v>0.312</v>
       </c>
       <c r="G5">
-        <v>0.223</v>
+        <v>0.18</v>
       </c>
       <c r="H5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
-        <v>14407</v>
+        <v>50021</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>2.319005275746444</v>
+        <v>5.579576795870956</v>
       </c>
       <c r="D6">
-        <v>160.8076271965465</v>
+        <v>88.74437334489292</v>
       </c>
       <c r="E6">
-        <v>0.1384149092917895</v>
+        <v>0.1030600830467635</v>
       </c>
       <c r="F6">
-        <v>0.244</v>
+        <v>0.415</v>
       </c>
       <c r="G6">
-        <v>0.412</v>
+        <v>0.522</v>
       </c>
       <c r="H6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
-        <v>75596</v>
+        <v>127441</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7">
-        <v>7.921046909511221</v>
+        <v>12.66761652990925</v>
       </c>
       <c r="D7">
-        <v>50.11157685734064</v>
+        <v>5.440012651552578</v>
       </c>
       <c r="E7">
-        <v>0.04313346006094358</v>
+        <v>0.00631756284385006</v>
       </c>
       <c r="F7">
-        <v>0.287</v>
+        <v>0.421</v>
       </c>
       <c r="G7">
-        <v>0.092</v>
+        <v>0.238</v>
       </c>
       <c r="H7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
-        <v>249113</v>
+        <v>154301</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>23.80706332040146</v>
+        <v>15.12673235600417</v>
       </c>
       <c r="D8">
-        <v>77.56436432956075</v>
+        <v>0.0160610900583665</v>
       </c>
       <c r="E8">
-        <v>0.06676340320493224</v>
+        <v>1.86519687147248E-05</v>
       </c>
       <c r="F8">
-        <v>0.354</v>
+        <v>0.421</v>
       </c>
       <c r="G8">
-        <v>0.768</v>
+        <v>0.76</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
-        <v>172041</v>
+        <v>255988</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9">
-        <v>16.75088405946373</v>
+        <v>24.43649077030476</v>
       </c>
       <c r="D9">
-        <v>3.065594989684187</v>
+        <v>89.04735805804688</v>
       </c>
       <c r="E9">
-        <v>0.002638706010529417</v>
+        <v>0.1034119434354576</v>
       </c>
       <c r="F9">
-        <v>0.357</v>
+        <v>0.525</v>
       </c>
       <c r="G9">
-        <v>0.914</v>
+        <v>0.263</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
-        <v>24598</v>
+        <v>39852</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10">
-        <v>3.25202275094128</v>
+        <v>4.64857348851581</v>
       </c>
       <c r="D10">
-        <v>138.0149694444013</v>
+        <v>107.1520308226577</v>
       </c>
       <c r="E10">
-        <v>0.11879616539088</v>
+        <v>0.1244371533538806</v>
       </c>
       <c r="F10">
-        <v>0.476</v>
+        <v>0.649</v>
       </c>
       <c r="G10">
-        <v>0.626</v>
+        <v>0.631</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
-        <v>219388</v>
+        <v>194409</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>21.08564790972866</v>
+        <v>18.79874343392728</v>
       </c>
       <c r="D11">
-        <v>37.03511048118477</v>
+        <v>14.43045167680564</v>
       </c>
       <c r="E11">
-        <v>0.03187791243010569</v>
+        <v>0.01675828553585119</v>
       </c>
       <c r="F11">
-        <v>0.507</v>
+        <v>0.666</v>
       </c>
       <c r="G11">
-        <v>0.647</v>
+        <v>0.874</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
-        <v>173240</v>
+        <v>149270</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12">
-        <v>16.86065620672686</v>
+        <v>14.66612879230038</v>
       </c>
       <c r="D12">
-        <v>3.462041519631195</v>
+        <v>0.1114699833308001</v>
       </c>
       <c r="E12">
-        <v>0.002979946730502171</v>
+        <v>0.0001294516520461151</v>
       </c>
       <c r="F12">
-        <v>0.51</v>
+        <v>0.666</v>
       </c>
       <c r="G12">
-        <v>0.9330000000000001</v>
+        <v>0.77</v>
       </c>
       <c r="H12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="I12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
-        <v>53352</v>
+        <v>86078</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13">
-        <v>5.884540117416829</v>
+        <v>8.880706332040145</v>
       </c>
       <c r="D13">
-        <v>83.09160887098319</v>
+        <v>37.44575499473358</v>
       </c>
       <c r="E13">
-        <v>0.0715209701510538</v>
+        <v>0.04348627945692843</v>
       </c>
       <c r="F13">
-        <v>0.582</v>
+        <v>0.71</v>
       </c>
       <c r="G13">
-        <v>0.822</v>
+        <v>0.585</v>
       </c>
       <c r="H13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
-        <v>140038</v>
+        <v>201295</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14">
-        <v>13.82091072429933</v>
+        <v>19.42917796775043</v>
       </c>
       <c r="D14">
-        <v>1.390251520072328</v>
+        <v>19.6176174700058</v>
       </c>
       <c r="E14">
-        <v>0.001196656784248082</v>
+        <v>0.02278221378363914</v>
       </c>
       <c r="F14">
-        <v>0.583</v>
+        <v>0.732</v>
       </c>
       <c r="G14">
-        <v>0.63</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
-        <v>61384</v>
+        <v>215078</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15">
-        <v>6.619894485071125</v>
+        <v>20.69105411931655</v>
       </c>
       <c r="D15">
-        <v>70.22616844134134</v>
+        <v>32.38809698898992</v>
       </c>
       <c r="E15">
-        <v>0.0604470627679714</v>
+        <v>0.03761275041561861</v>
       </c>
       <c r="F15">
-        <v>0.644</v>
+        <v>0.77</v>
       </c>
       <c r="G15">
-        <v>0.725</v>
+        <v>0.929</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>18</v>
+      </c>
+      <c r="I15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
-        <v>18672</v>
+        <v>43305</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16">
-        <v>2.709479177395544</v>
+        <v>4.964706286263604</v>
       </c>
       <c r="D16">
-        <v>151.0569020908737</v>
+        <v>100.7071199209572</v>
       </c>
       <c r="E16">
-        <v>0.1300219881688301</v>
+        <v>0.1169525881051423</v>
       </c>
       <c r="F16">
-        <v>0.774</v>
+        <v>0.887</v>
       </c>
       <c r="G16">
-        <v>0.921</v>
+        <v>0.349</v>
       </c>
       <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17">
-        <v>87519</v>
+        <v>132791</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17">
-        <v>9.012634325539876</v>
+        <v>13.15742552728854</v>
       </c>
       <c r="D17">
-        <v>35.84854771970333</v>
+        <v>3.395080687487915</v>
       </c>
       <c r="E17">
-        <v>0.03085658042078048</v>
+        <v>0.003942754728157687</v>
       </c>
       <c r="F17">
-        <v>0.805</v>
+        <v>0.891</v>
       </c>
       <c r="G17">
-        <v>0.982</v>
+        <v>0.376</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
-        <v>39868</v>
+        <v>101740</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18">
-        <v>4.650038337853767</v>
+        <v>10.31461072773257</v>
       </c>
       <c r="D18">
-        <v>107.1217064078968</v>
+        <v>21.95287263267869</v>
       </c>
       <c r="E18">
-        <v>0.09220483837814611</v>
+        <v>0.02549417829394239</v>
       </c>
       <c r="F18">
-        <v>0.897</v>
+        <v>0.916</v>
       </c>
       <c r="G18">
-        <v>0.195</v>
+        <v>0.908</v>
       </c>
       <c r="H18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>17</v>
+      </c>
+      <c r="I18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
-        <v>45539</v>
+        <v>64886</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="C19">
-        <v>5.169235875075817</v>
+        <v>6.940513383916412</v>
       </c>
       <c r="D19">
-        <v>96.64392327989634</v>
+        <v>64.95532451483051</v>
       </c>
       <c r="E19">
-        <v>0.08318610321909405</v>
+        <v>0.07543352763122704</v>
       </c>
       <c r="F19">
-        <v>0.98</v>
+        <v>0.992</v>
       </c>
       <c r="G19">
-        <v>0.834</v>
+        <v>0.99</v>
       </c>
       <c r="H19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>18</v>
+      </c>
+      <c r="I19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
-        <v>205690</v>
+        <v>123931</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
       <c r="C20">
-        <v>19.83155377027042</v>
+        <v>12.34626520639498</v>
       </c>
       <c r="D20">
-        <v>23.34391183501436</v>
+        <v>7.042308354789869</v>
       </c>
       <c r="E20">
-        <v>0.02009323497578748</v>
+        <v>0.008178331273633677</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>0.418</v>
+        <v>0.927</v>
       </c>
       <c r="H20" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="I20" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Description foreach col
</commit_message>
<xml_diff>
--- a/GA.xlsx
+++ b/GA.xlsx
@@ -16,138 +16,219 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="44">
-  <si>
-    <t>111000010010110100</t>
-  </si>
-  <si>
-    <t>001110111000111011</t>
-  </si>
-  <si>
-    <t>010111110001111110</t>
-  </si>
-  <si>
-    <t>001100111110101011</t>
-  </si>
-  <si>
-    <t>010110101101001000</t>
-  </si>
-  <si>
-    <t>111101001010100101</t>
-  </si>
-  <si>
-    <t>101110001100011001</t>
-  </si>
-  <si>
-    <t>000111100011000000</t>
-  </si>
-  <si>
-    <t>001101110100011011</t>
-  </si>
-  <si>
-    <t>101011001010001111</t>
-  </si>
-  <si>
-    <t>001101100011000101</t>
-  </si>
-  <si>
-    <t>111000100110101000</t>
-  </si>
-  <si>
-    <t>010110001111110000</t>
-  </si>
-  <si>
-    <t>101000111010111110</t>
-  </si>
-  <si>
-    <t>011101000101101001</t>
-  </si>
-  <si>
-    <t>010100110000000101</t>
-  </si>
-  <si>
-    <t>010011000100000111</t>
-  </si>
-  <si>
-    <t>100111100010101011</t>
-  </si>
-  <si>
-    <t>110101011000111000</t>
-  </si>
-  <si>
-    <t>000011100101000111</t>
-  </si>
-  <si>
-    <t>000011000101000111</t>
-  </si>
-  <si>
-    <t>111111100011000000</t>
-  </si>
-  <si>
-    <t>000000100110101000</t>
-  </si>
-  <si>
-    <t>111001010010110100</t>
-  </si>
-  <si>
-    <t>011101100011000101</t>
-  </si>
-  <si>
-    <t>000011000100000111</t>
-  </si>
-  <si>
-    <t>001100100101000111</t>
-  </si>
-  <si>
-    <t>000011111110101011</t>
-  </si>
-  <si>
-    <t>000111100101000111</t>
-  </si>
-  <si>
-    <t>000011100011000000</t>
-  </si>
-  <si>
-    <t>110101011100111000</t>
-  </si>
-  <si>
-    <t>100111100101111000</t>
-  </si>
-  <si>
-    <t>110101011000000111</t>
-  </si>
-  <si>
-    <t>000000100110111011</t>
-  </si>
-  <si>
-    <t>001110111000101000</t>
-  </si>
-  <si>
-    <t>000111100101111000</t>
-  </si>
-  <si>
-    <t>001000100110101000</t>
-  </si>
-  <si>
-    <t>000100111110101011</t>
-  </si>
-  <si>
-    <t>001100111110111011</t>
-  </si>
-  <si>
-    <t>011110111000101011</t>
-  </si>
-  <si>
-    <t>000000100011000001</t>
-  </si>
-  <si>
-    <t>000111100110101000</t>
-  </si>
-  <si>
-    <t>001110111000101011</t>
-  </si>
-  <si>
-    <t>000000100011000000</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="71">
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>Binário</t>
+  </si>
+  <si>
+    <t>Valor Real</t>
+  </si>
+  <si>
+    <t>Função Avaliação</t>
+  </si>
+  <si>
+    <t>Probabilidade de ser Selecionada</t>
+  </si>
+  <si>
+    <t>Segmento da Roleta</t>
+  </si>
+  <si>
+    <t>Aleatório Roleta</t>
+  </si>
+  <si>
+    <t>Individuo Selecionado</t>
+  </si>
+  <si>
+    <t>Probabilidade de Recombinação</t>
+  </si>
+  <si>
+    <t>Ponto de Corte Aleatório</t>
+  </si>
+  <si>
+    <t>Recombinação</t>
+  </si>
+  <si>
+    <t>Mutação</t>
+  </si>
+  <si>
+    <t>011111100111110100</t>
+  </si>
+  <si>
+    <t>000011001010010001</t>
+  </si>
+  <si>
+    <t>010101000110101100</t>
+  </si>
+  <si>
+    <t>010101010100010100</t>
+  </si>
+  <si>
+    <t>110111110110011110</t>
+  </si>
+  <si>
+    <t>110010100111100100</t>
+  </si>
+  <si>
+    <t>011001110100000011</t>
+  </si>
+  <si>
+    <t>001110011100001100</t>
+  </si>
+  <si>
+    <t>001111011010101000</t>
+  </si>
+  <si>
+    <t>010011110111100010</t>
+  </si>
+  <si>
+    <t>101000001010000110</t>
+  </si>
+  <si>
+    <t>000010100110010110</t>
+  </si>
+  <si>
+    <t>110111101000000101</t>
+  </si>
+  <si>
+    <t>100110111111001111</t>
+  </si>
+  <si>
+    <t>011111110110011001</t>
+  </si>
+  <si>
+    <t>000010001010000101</t>
+  </si>
+  <si>
+    <t>010001001100011101</t>
+  </si>
+  <si>
+    <t>100110111010111101</t>
+  </si>
+  <si>
+    <t>001110110000110010</t>
+  </si>
+  <si>
+    <t>000111111000001011</t>
+  </si>
+  <si>
+    <t>000010001010000001</t>
+  </si>
+  <si>
+    <t>011001110100001000</t>
+  </si>
+  <si>
+    <t>001111011010100011</t>
+  </si>
+  <si>
+    <t>110111110110011011</t>
+  </si>
+  <si>
+    <t>000111111000001110</t>
+  </si>
+  <si>
+    <t>000010100110010001</t>
+  </si>
+  <si>
+    <t>000011001010010110</t>
+  </si>
+  <si>
+    <t>000010000010000100</t>
+  </si>
+  <si>
+    <t>010101010100010101</t>
+  </si>
+  <si>
+    <t>010101000110101110</t>
+  </si>
+  <si>
+    <t>000010100110010100</t>
+  </si>
+  <si>
+    <t>001110110000110001</t>
+  </si>
+  <si>
+    <t>000011001010010010</t>
+  </si>
+  <si>
+    <t>010011110111100000</t>
+  </si>
+  <si>
+    <t>001110011100001110</t>
+  </si>
+  <si>
+    <t>000010001010000100</t>
+  </si>
+  <si>
+    <t>110110011100001110</t>
+  </si>
+  <si>
+    <t>000111110110011011</t>
+  </si>
+  <si>
+    <t>000010100111010110</t>
+  </si>
+  <si>
+    <t>000011001010100011</t>
+  </si>
+  <si>
+    <t>001111011010010010</t>
+  </si>
+  <si>
+    <t>011001110100010101</t>
+  </si>
+  <si>
+    <t>010101010100001000</t>
+  </si>
+  <si>
+    <t>010011110110010110</t>
+  </si>
+  <si>
+    <t>000010100111100000</t>
+  </si>
+  <si>
+    <t>001110010100010101</t>
+  </si>
+  <si>
+    <t>010101011100001110</t>
+  </si>
+  <si>
+    <t>000011001010010101</t>
+  </si>
+  <si>
+    <t>111110011100001110</t>
+  </si>
+  <si>
+    <t>110111110100010101</t>
+  </si>
+  <si>
+    <t>010101010110011011</t>
+  </si>
+  <si>
+    <t>110101010100010101</t>
+  </si>
+  <si>
+    <t>011110011100001110</t>
+  </si>
+  <si>
+    <t>001111010010010101</t>
+  </si>
+  <si>
+    <t>110101010100010010</t>
+  </si>
+  <si>
+    <t>110111011010010010</t>
+  </si>
+  <si>
+    <t>001111110110011110</t>
+  </si>
+  <si>
+    <t>001111011010010101</t>
+  </si>
+  <si>
+    <t>010101010100010010</t>
   </si>
 </sst>
 </file>
@@ -479,770 +560,822 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:L21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="2" spans="1:12">
       <c r="A2">
-        <v>230580</v>
+        <v>129524</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>22.11031002162942</v>
+        <v>12.85832160309449</v>
       </c>
       <c r="D2">
-        <v>50.55650860368372</v>
+        <v>4.58678635577174</v>
       </c>
       <c r="E2">
-        <v>0.04971943980357146</v>
+        <v>0.003936273833947527</v>
       </c>
       <c r="F2">
-        <v>0.05</v>
+        <v>0.004</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>60987</v>
+        <v>12945</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>6.583547910873072</v>
+        <v>2.185154667490644</v>
       </c>
       <c r="D3">
-        <v>70.83666576856902</v>
+        <v>164.2202608961368</v>
       </c>
       <c r="E3">
-        <v>0.06966381652607745</v>
+        <v>0.1409300250394458</v>
       </c>
       <c r="F3">
-        <v>0.119</v>
+        <v>0.145</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="L3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>97406</v>
+        <v>86444</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>9.917819663313534</v>
+        <v>8.914214760645907</v>
       </c>
       <c r="D4">
-        <v>25.82855697460257</v>
+        <v>37.03678197954016</v>
       </c>
       <c r="E4">
-        <v>0.02540091116217425</v>
+        <v>0.03178410863114076</v>
       </c>
       <c r="F4">
-        <v>0.145</v>
+        <v>0.177</v>
       </c>
       <c r="G4">
-        <v>0.947</v>
+        <v>0.284</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4">
-        <v>0.98</v>
+        <v>0.6</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>53163</v>
+        <v>87316</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>5.867236584612215</v>
+        <v>8.99404904956455</v>
       </c>
       <c r="D5">
-        <v>83.40736760144556</v>
+        <v>36.07144681903648</v>
       </c>
       <c r="E5">
-        <v>0.08202638408326059</v>
+        <v>0.03095568035073945</v>
       </c>
       <c r="F5">
-        <v>0.227</v>
+        <v>0.208</v>
       </c>
       <c r="G5">
-        <v>0.368</v>
+        <v>0.395</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I5">
-        <v>0.98</v>
+        <v>0.6</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K5" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="L5" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
-        <v>93000</v>
+        <v>228766</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>9.514436776873691</v>
+        <v>21.94423272793857</v>
       </c>
       <c r="D6">
-        <v>30.0914038749159</v>
+        <v>48.2223681797731</v>
       </c>
       <c r="E6">
-        <v>0.0295931777111449</v>
+        <v>0.04138331968267301</v>
       </c>
       <c r="F6">
-        <v>0.256</v>
+        <v>0.249</v>
       </c>
       <c r="G6">
-        <v>0.819</v>
+        <v>0.238</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I6">
-        <v>0.93</v>
+        <v>0.05</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
-        <v>250533</v>
+        <v>207332</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>23.93706869914512</v>
+        <v>19.98188393357824</v>
       </c>
       <c r="D7">
-        <v>79.87119693323949</v>
+        <v>24.81916752764498</v>
       </c>
       <c r="E7">
-        <v>0.07854876212065108</v>
+        <v>0.02129923483279212</v>
       </c>
       <c r="F7">
-        <v>0.335</v>
+        <v>0.27</v>
       </c>
       <c r="G7">
-        <v>0.833</v>
+        <v>0.98</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I7">
-        <v>0.93</v>
+        <v>0.05</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="L7" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>189209</v>
+        <v>105731</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C8">
-        <v>18.32266739909133</v>
+        <v>10.67999908446916</v>
       </c>
       <c r="D8">
-        <v>11.04011864498437</v>
+        <v>18.66240791018727</v>
       </c>
       <c r="E8">
-        <v>0.0108573263770353</v>
+        <v>0.01601564630166115</v>
       </c>
       <c r="F8">
-        <v>0.346</v>
+        <v>0.286</v>
       </c>
       <c r="G8">
-        <v>0.677</v>
+        <v>0.239</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I8">
-        <v>0.15</v>
+        <v>0.79</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>30912</v>
+        <v>59148</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>3.830088920932468</v>
+        <v>6.415181790091667</v>
       </c>
       <c r="D9">
-        <v>124.7669135142756</v>
+        <v>73.69910369717371</v>
       </c>
       <c r="E9">
-        <v>0.1227011361599135</v>
+        <v>0.06324686413691927</v>
       </c>
       <c r="F9">
-        <v>0.469</v>
+        <v>0.35</v>
       </c>
       <c r="G9">
-        <v>0.444</v>
+        <v>0.09</v>
       </c>
       <c r="H9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I9">
-        <v>0.15</v>
+        <v>0.79</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K9" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L9" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>56603</v>
+        <v>63144</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>6.182179192272919</v>
+        <v>6.781027912246369</v>
       </c>
       <c r="D10">
-        <v>77.75396379718467</v>
+        <v>67.55150217927329</v>
       </c>
       <c r="E10">
-        <v>0.07646658420992142</v>
+        <v>0.05797113487475353</v>
       </c>
       <c r="F10">
-        <v>0.545</v>
+        <v>0.408</v>
       </c>
       <c r="G10">
-        <v>0.65</v>
+        <v>0.59</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="I10">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="J10">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K10" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="L10" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11">
-        <v>176783</v>
+        <v>81378</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C11">
-        <v>17.18502878200066</v>
+        <v>8.450406839015347</v>
       </c>
       <c r="D11">
-        <v>4.774350778171306</v>
+        <v>42.89717057441694</v>
       </c>
       <c r="E11">
-        <v>0.004695301409700721</v>
+        <v>0.03681335841378006</v>
       </c>
       <c r="F11">
-        <v>0.55</v>
+        <v>0.444</v>
       </c>
       <c r="G11">
-        <v>0.004</v>
+        <v>0.144</v>
       </c>
       <c r="H11" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I11">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="J11">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K11" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="L11" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12">
-        <v>55493</v>
+        <v>164486</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C12">
-        <v>6.080555269452169</v>
+        <v>16.05920051269727</v>
       </c>
       <c r="D12">
-        <v>79.55649430129746</v>
+        <v>1.121905726098152</v>
       </c>
       <c r="E12">
-        <v>0.07823927004936262</v>
+        <v>0.0009627935140774683</v>
       </c>
       <c r="F12">
-        <v>0.628</v>
+        <v>0.445</v>
       </c>
       <c r="G12">
-        <v>0.83</v>
+        <v>0.767</v>
       </c>
       <c r="H12" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="I12">
-        <v>0.96</v>
+        <v>0.3</v>
       </c>
       <c r="J12">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K12" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="L12" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13">
-        <v>231848</v>
+        <v>10646</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C13">
-        <v>22.22639933166249</v>
+        <v>1.974674128242982</v>
       </c>
       <c r="D13">
-        <v>52.22084730065206</v>
+        <v>169.6591140654627</v>
       </c>
       <c r="E13">
-        <v>0.05135622189043105</v>
+        <v>0.1455975228814066</v>
       </c>
       <c r="F13">
-        <v>0.679</v>
+        <v>0.591</v>
       </c>
       <c r="G13">
-        <v>0.8169999999999999</v>
+        <v>0.203</v>
       </c>
       <c r="H13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I13">
-        <v>0.96</v>
+        <v>0.3</v>
       </c>
       <c r="J13">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K13" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="L13" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14">
-        <v>91120</v>
+        <v>227845</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C14">
-        <v>9.342316979663771</v>
+        <v>21.85991233792243</v>
       </c>
       <c r="D14">
-        <v>32.00937715860088</v>
+        <v>47.05839728398039</v>
       </c>
       <c r="E14">
-        <v>0.03147939493335405</v>
+        <v>0.04038442681407015</v>
       </c>
       <c r="F14">
-        <v>0.711</v>
+        <v>0.631</v>
       </c>
       <c r="G14">
-        <v>0.791</v>
+        <v>0.176</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I14">
-        <v>0.11</v>
+        <v>0.4</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="K14" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="L14" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15">
-        <v>167614</v>
+        <v>159695</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C15">
-        <v>16.34557855826781</v>
+        <v>15.62056968906284</v>
       </c>
       <c r="D15">
-        <v>1.810581656470089</v>
+        <v>0.385106738983548</v>
       </c>
       <c r="E15">
-        <v>0.001780603688122483</v>
+        <v>0.0003304896854483531</v>
       </c>
       <c r="F15">
-        <v>0.713</v>
+        <v>0.632</v>
       </c>
       <c r="G15">
-        <v>0.5580000000000001</v>
+        <v>0.504</v>
       </c>
       <c r="H15" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="I15">
-        <v>0.11</v>
+        <v>0.4</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="K15" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="L15" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16">
-        <v>119145</v>
+        <v>130457</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C16">
-        <v>11.90809214817867</v>
+        <v>12.9437406301141</v>
       </c>
       <c r="D16">
-        <v>9.559894164154418</v>
+        <v>4.228202596243568</v>
       </c>
       <c r="E16">
-        <v>0.009401610110168027</v>
+        <v>0.003628545555273036</v>
       </c>
       <c r="F16">
-        <v>0.722</v>
+        <v>0.635</v>
       </c>
       <c r="G16">
-        <v>0.208</v>
+        <v>0.852</v>
       </c>
       <c r="H16" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="I16">
-        <v>0.65</v>
+        <v>0.33</v>
       </c>
       <c r="J16">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K16" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="L16" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17">
-        <v>84997</v>
+        <v>8837</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C17">
-        <v>8.781737448644442</v>
+        <v>1.809054599970245</v>
       </c>
       <c r="D17">
-        <v>38.66678915759093</v>
+        <v>174.0010405465661</v>
       </c>
       <c r="E17">
-        <v>0.03802657954465932</v>
+        <v>0.1493236636411534</v>
       </c>
       <c r="F17">
-        <v>0.76</v>
+        <v>0.785</v>
       </c>
       <c r="G17">
-        <v>0.886</v>
+        <v>0.14</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I17">
-        <v>0.65</v>
+        <v>0.33</v>
       </c>
       <c r="J17">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K17" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="L17" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18">
-        <v>78087</v>
+        <v>70429</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C18">
-        <v>8.149105640814364</v>
+        <v>7.447992126434809</v>
       </c>
       <c r="D18">
-        <v>46.93475352072157</v>
+        <v>57.03282292239064</v>
       </c>
       <c r="E18">
-        <v>0.04615765045529564</v>
+        <v>0.04894424791838746</v>
       </c>
       <c r="F18">
-        <v>0.806</v>
+        <v>0.834</v>
       </c>
       <c r="G18">
-        <v>0.372</v>
+        <v>0.976</v>
       </c>
       <c r="H18" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="I18">
-        <v>0.06</v>
+        <v>0.38</v>
       </c>
       <c r="J18">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19">
-        <v>161963</v>
+        <v>159421</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C19">
-        <v>15.82821208271821</v>
+        <v>15.59548414415033</v>
       </c>
       <c r="D19">
-        <v>0.6859352539604348</v>
+        <v>0.3546013659344507</v>
       </c>
       <c r="E19">
-        <v>0.0006745781603666434</v>
+        <v>0.0003043106807129633</v>
       </c>
       <c r="F19">
-        <v>0.8070000000000001</v>
+        <v>0.834</v>
       </c>
       <c r="G19">
-        <v>0.98</v>
+        <v>0.547</v>
       </c>
       <c r="H19" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I19">
-        <v>0.06</v>
+        <v>0.38</v>
       </c>
       <c r="J19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20">
-        <v>218680</v>
+        <v>60466</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C20">
-        <v>21.02082832652407</v>
+        <v>6.535848754305856</v>
       </c>
       <c r="D20">
-        <v>36.25037373747465</v>
+        <v>71.64185630998573</v>
       </c>
       <c r="E20">
-        <v>0.03565017293868299</v>
+        <v>0.06148138206907561</v>
       </c>
       <c r="F20">
-        <v>0.842</v>
+        <v>0.895</v>
       </c>
       <c r="G20">
-        <v>0.064</v>
+        <v>0.41</v>
       </c>
       <c r="H20" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="I20">
-        <v>0.19</v>
+        <v>0.64</v>
       </c>
       <c r="J20">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="K20" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="L20" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21">
-        <v>14663</v>
+        <v>32267</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C21">
-        <v>2.342442865153752</v>
+        <v>3.954143349240681</v>
       </c>
       <c r="D21">
-        <v>160.2137526218972</v>
+        <v>122.0109491491239</v>
       </c>
       <c r="E21">
-        <v>0.1575610786661066</v>
+        <v>0.1047069711425423</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21">
-        <v>0.183</v>
+        <v>0.294</v>
       </c>
       <c r="H21" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="I21">
-        <v>0.19</v>
+        <v>0.64</v>
       </c>
       <c r="J21">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="K21" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="L21" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1252,770 +1385,822 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:L21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="2" spans="1:12">
       <c r="A2">
-        <v>14663</v>
+        <v>8837</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C2">
-        <v>2.342442865153752</v>
+        <v>1.809054599970245</v>
       </c>
       <c r="D2">
-        <v>160.2137526218972</v>
+        <v>174.0010405465661</v>
       </c>
       <c r="E2">
-        <v>0.08175724186360812</v>
+        <v>0.07882900972737399</v>
       </c>
       <c r="F2">
-        <v>0.082</v>
+        <v>0.079</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>30912</v>
+        <v>10646</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C3">
-        <v>3.830088920932468</v>
+        <v>1.974674128242982</v>
       </c>
       <c r="D3">
-        <v>124.7669135142756</v>
+        <v>169.6591140654627</v>
       </c>
       <c r="E3">
-        <v>0.06366868360443324</v>
+        <v>0.07686195387679219</v>
       </c>
       <c r="F3">
-        <v>0.145</v>
+        <v>0.156</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>14663</v>
+        <v>105736</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C4">
-        <v>2.342442865153752</v>
+        <v>10.68045684988727</v>
       </c>
       <c r="D4">
-        <v>160.2137526218972</v>
+        <v>18.65845302568577</v>
       </c>
       <c r="E4">
-        <v>0.08175724186360812</v>
+        <v>0.008452980341033714</v>
       </c>
       <c r="F4">
-        <v>0.227</v>
+        <v>0.164</v>
       </c>
       <c r="G4">
-        <v>0.985</v>
+        <v>0.8110000000000001</v>
       </c>
       <c r="H4" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I4">
-        <v>0.99</v>
+        <v>0.85</v>
       </c>
       <c r="J4">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="L4" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>30912</v>
+        <v>63139</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C5">
-        <v>3.830088920932468</v>
+        <v>6.780570146828257</v>
       </c>
       <c r="D5">
-        <v>124.7669135142756</v>
+        <v>67.55902711121085</v>
       </c>
       <c r="E5">
-        <v>0.06366868360443324</v>
+        <v>0.03060677791691897</v>
       </c>
       <c r="F5">
-        <v>0.291</v>
+        <v>0.195</v>
       </c>
       <c r="G5">
-        <v>0.639</v>
+        <v>0.435</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="I5">
-        <v>0.99</v>
+        <v>0.85</v>
       </c>
       <c r="J5">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="L5" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
-        <v>218680</v>
+        <v>228763</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C6">
-        <v>21.02082832652407</v>
+        <v>21.9439580686877</v>
       </c>
       <c r="D6">
-        <v>36.25037373747465</v>
+        <v>48.218553659693</v>
       </c>
       <c r="E6">
-        <v>0.01849860280281479</v>
+        <v>0.02184481669500485</v>
       </c>
       <c r="F6">
-        <v>0.309</v>
+        <v>0.217</v>
       </c>
       <c r="G6">
-        <v>0.534</v>
+        <v>0.128</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="I6">
-        <v>0.66</v>
+        <v>0.13</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="L6" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
-        <v>218680</v>
+        <v>32270</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C7">
-        <v>21.02082832652407</v>
+        <v>3.954418008491548</v>
       </c>
       <c r="D7">
-        <v>36.25037373747465</v>
+        <v>122.0048815311358</v>
       </c>
       <c r="E7">
-        <v>0.01849860280281479</v>
+        <v>0.05527279585682234</v>
       </c>
       <c r="F7">
-        <v>0.328</v>
+        <v>0.272</v>
       </c>
       <c r="G7">
-        <v>0.607</v>
+        <v>0.598</v>
       </c>
       <c r="H7" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="I7">
-        <v>0.66</v>
+        <v>0.13</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="L7" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>260288</v>
+        <v>228766</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>24.83016902988064</v>
+        <v>21.94423272793857</v>
       </c>
       <c r="D8">
-        <v>96.63222315602441</v>
+        <v>48.2223681797731</v>
       </c>
       <c r="E8">
-        <v>0.04931152233248082</v>
+        <v>0.02184654481593766</v>
       </c>
       <c r="F8">
-        <v>0.377</v>
+        <v>0.294</v>
       </c>
       <c r="G8">
-        <v>0.666</v>
+        <v>0.837</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="I8">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="L8" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>2472</v>
+        <v>12945</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>1.22631922271432</v>
+        <v>2.185154667490644</v>
       </c>
       <c r="D9">
-        <v>189.714282154569</v>
+        <v>164.2202608961368</v>
       </c>
       <c r="E9">
-        <v>0.09681139226353781</v>
+        <v>0.07439794901771887</v>
       </c>
       <c r="F9">
-        <v>0.474</v>
+        <v>0.368</v>
       </c>
       <c r="G9">
-        <v>0.666</v>
+        <v>0.624</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I9">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
       <c r="J9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>230580</v>
+        <v>10641</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C10">
-        <v>22.11031002162942</v>
+        <v>1.97421636282487</v>
       </c>
       <c r="D10">
-        <v>50.55650860368372</v>
+        <v>169.6710393624993</v>
       </c>
       <c r="E10">
-        <v>0.0257990380603945</v>
+        <v>0.07686735648446136</v>
       </c>
       <c r="F10">
-        <v>0.5</v>
+        <v>0.445</v>
       </c>
       <c r="G10">
-        <v>0.833</v>
+        <v>0.22</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="I10">
-        <v>0.9</v>
+        <v>0.84</v>
       </c>
       <c r="J10">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K10" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="L10" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11">
-        <v>231848</v>
+        <v>12950</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C11">
-        <v>22.22639933166249</v>
+        <v>2.185612432908756</v>
       </c>
       <c r="D11">
-        <v>52.22084730065206</v>
+        <v>164.2085287196227</v>
       </c>
       <c r="E11">
-        <v>0.02664835180009656</v>
+        <v>0.07439263390090319</v>
       </c>
       <c r="F11">
-        <v>0.526</v>
+        <v>0.519</v>
       </c>
       <c r="G11">
-        <v>0.8110000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I11">
-        <v>0.9</v>
+        <v>0.84</v>
       </c>
       <c r="J11">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K11" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="L11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12">
-        <v>218680</v>
+        <v>8836</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="C12">
-        <v>21.02082832652407</v>
+        <v>1.808963046886623</v>
       </c>
       <c r="D12">
-        <v>36.25037373747465</v>
+        <v>174.0034558984026</v>
       </c>
       <c r="E12">
-        <v>0.01849860280281479</v>
+        <v>0.07883010397251652</v>
       </c>
       <c r="F12">
-        <v>0.545</v>
+        <v>0.598</v>
       </c>
       <c r="G12">
-        <v>0.7</v>
+        <v>0.275</v>
       </c>
       <c r="H12" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="I12">
-        <v>0.95</v>
+        <v>0.49</v>
       </c>
       <c r="J12">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="K12" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="L12" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13">
-        <v>218680</v>
+        <v>87317</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C13">
-        <v>21.02082832652407</v>
+        <v>8.994140602648173</v>
       </c>
       <c r="D13">
-        <v>36.25037373747465</v>
+        <v>36.07034710075925</v>
       </c>
       <c r="E13">
-        <v>0.01849860280281479</v>
+        <v>0.01634122263604831</v>
       </c>
       <c r="F13">
-        <v>0.5629999999999999</v>
+        <v>0.615</v>
       </c>
       <c r="G13">
-        <v>0.272</v>
+        <v>0.145</v>
       </c>
       <c r="H13" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="I13">
-        <v>0.95</v>
+        <v>0.49</v>
       </c>
       <c r="J13">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="K13" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="L13" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14">
-        <v>121029</v>
+        <v>86446</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C14">
-        <v>12.08057815772307</v>
+        <v>8.91439786681315</v>
       </c>
       <c r="D14">
-        <v>8.523023893163597</v>
+        <v>37.03455332344834</v>
       </c>
       <c r="E14">
-        <v>0.004349307811840428</v>
+        <v>0.01677804428647523</v>
       </c>
       <c r="F14">
-        <v>0.5679999999999999</v>
+        <v>0.631</v>
       </c>
       <c r="G14">
-        <v>0.859</v>
+        <v>0.042</v>
       </c>
       <c r="H14" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I14">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="J14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K14" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="L14" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15">
-        <v>12551</v>
+        <v>10644</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C15">
-        <v>2.149082752543459</v>
+        <v>1.974491022075737</v>
       </c>
       <c r="D15">
-        <v>165.146074100976</v>
+        <v>169.6638841339856</v>
       </c>
       <c r="E15">
-        <v>0.08427421056020805</v>
+        <v>0.07686411489707577</v>
       </c>
       <c r="F15">
-        <v>0.652</v>
+        <v>0.708</v>
       </c>
       <c r="G15">
-        <v>0.237</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="H15" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="I15">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="J15">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K15" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="L15" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16">
-        <v>51527</v>
+        <v>60465</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C16">
-        <v>5.717455739806136</v>
+        <v>6.535757201222234</v>
       </c>
       <c r="D16">
-        <v>86.16562794245806</v>
+        <v>71.64340615666127</v>
       </c>
       <c r="E16">
-        <v>0.04397040808754133</v>
+        <v>0.03245715510140442</v>
       </c>
       <c r="F16">
-        <v>0.696</v>
+        <v>0.741</v>
       </c>
       <c r="G16">
-        <v>0.109</v>
+        <v>0.871</v>
       </c>
       <c r="H16" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="I16">
-        <v>0.79</v>
+        <v>0.1</v>
       </c>
       <c r="J16">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="K16" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="L16" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17">
-        <v>16299</v>
+        <v>12946</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C17">
-        <v>2.492223709959831</v>
+        <v>2.185246220574267</v>
       </c>
       <c r="D17">
-        <v>156.444467721691</v>
+        <v>164.2179144273061</v>
       </c>
       <c r="E17">
-        <v>0.07983377192300777</v>
+        <v>0.07439688597916634</v>
       </c>
       <c r="F17">
-        <v>0.776</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="G17">
-        <v>0.539</v>
+        <v>0.068</v>
       </c>
       <c r="H17" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="I17">
-        <v>0.79</v>
+        <v>0.1</v>
       </c>
       <c r="J17">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="K17" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="L17" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18">
-        <v>31047</v>
+        <v>10646</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C18">
-        <v>3.842448587221478</v>
+        <v>1.974674128242982</v>
       </c>
       <c r="D18">
-        <v>124.490953528796</v>
+        <v>169.6591140654627</v>
       </c>
       <c r="E18">
-        <v>0.06352786094153251</v>
+        <v>0.07686195387679219</v>
       </c>
       <c r="F18">
-        <v>0.839</v>
+        <v>0.892</v>
       </c>
       <c r="G18">
-        <v>0.8120000000000001</v>
+        <v>0.435</v>
       </c>
       <c r="H18" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="I18">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
       <c r="J18">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="K18" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="L18" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19">
-        <v>14528</v>
+        <v>32267</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C19">
-        <v>2.330083198864742</v>
+        <v>3.954143349240681</v>
       </c>
       <c r="D19">
-        <v>160.5267917476895</v>
+        <v>122.0109491491239</v>
       </c>
       <c r="E19">
-        <v>0.08191698604974285</v>
+        <v>0.0552755447157711</v>
       </c>
       <c r="F19">
-        <v>0.921</v>
+        <v>0.947</v>
       </c>
       <c r="G19">
-        <v>0.632</v>
+        <v>0.602</v>
       </c>
       <c r="H19" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="I19">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
       <c r="J19">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="K19" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="L19" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20">
-        <v>53163</v>
+        <v>81376</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C20">
-        <v>5.867236584612215</v>
+        <v>8.450223732848102</v>
       </c>
       <c r="D20">
-        <v>83.40736760144556</v>
+        <v>42.89956914974626</v>
       </c>
       <c r="E20">
-        <v>0.04256286501378815</v>
+        <v>0.01943511684288165</v>
       </c>
       <c r="F20">
-        <v>0.964</v>
+        <v>0.967</v>
       </c>
       <c r="G20">
-        <v>0.471</v>
+        <v>0.91</v>
       </c>
       <c r="H20" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="I20">
-        <v>0.97</v>
+        <v>0.64</v>
       </c>
       <c r="J20">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="K20" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="L20" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21">
-        <v>60987</v>
+        <v>59150</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="C21">
-        <v>6.583547910873072</v>
+        <v>6.415364896258912</v>
       </c>
       <c r="D21">
-        <v>70.83666576856902</v>
+        <v>73.69595986438378</v>
       </c>
       <c r="E21">
-        <v>0.03614802300848752</v>
+        <v>0.03338703905890129</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21">
-        <v>0.224</v>
+        <v>0.869</v>
       </c>
       <c r="H21" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I21">
-        <v>0.97</v>
+        <v>0.64</v>
       </c>
       <c r="J21">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="K21" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="L21" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2025,770 +2210,822 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:L21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="2" spans="1:12">
       <c r="A2">
-        <v>60987</v>
+        <v>12946</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C2">
-        <v>6.583547910873072</v>
+        <v>2.185246220574267</v>
       </c>
       <c r="D2">
-        <v>70.83666576856902</v>
+        <v>164.2179144273061</v>
       </c>
       <c r="E2">
-        <v>0.03304847452272566</v>
+        <v>0.08251820262989461</v>
       </c>
       <c r="F2">
-        <v>0.033</v>
+        <v>0.083</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K2" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="L2" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>2472</v>
+        <v>87317</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C3">
-        <v>1.22631922271432</v>
+        <v>8.994140602648173</v>
       </c>
       <c r="D3">
-        <v>189.714282154569</v>
+        <v>36.07034710075925</v>
       </c>
       <c r="E3">
-        <v>0.08851020234163003</v>
+        <v>0.0181250640124812</v>
       </c>
       <c r="F3">
-        <v>0.122</v>
+        <v>0.101</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>60987</v>
+        <v>228766</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>6.583547910873072</v>
+        <v>21.94423272793857</v>
       </c>
       <c r="D4">
-        <v>70.83666576856902</v>
+        <v>48.2223681797731</v>
       </c>
       <c r="E4">
-        <v>0.03304847452272566</v>
+        <v>0.02423135845214604</v>
       </c>
       <c r="F4">
-        <v>0.155</v>
+        <v>0.125</v>
       </c>
       <c r="G4">
-        <v>0.453</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="I4">
-        <v>0.6899999999999999</v>
+        <v>0.08</v>
       </c>
       <c r="J4">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K4" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>2472</v>
+        <v>10641</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C5">
-        <v>1.22631922271432</v>
+        <v>1.97421636282487</v>
       </c>
       <c r="D5">
-        <v>189.714282154569</v>
+        <v>169.6710393624993</v>
       </c>
       <c r="E5">
-        <v>0.08851020234163003</v>
+        <v>0.08525835476212497</v>
       </c>
       <c r="F5">
-        <v>0.243</v>
+        <v>0.21</v>
       </c>
       <c r="G5">
-        <v>0.044</v>
+        <v>0.609</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="I5">
-        <v>0.6899999999999999</v>
+        <v>0.08</v>
       </c>
       <c r="J5">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K5" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="L5" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
-        <v>53163</v>
+        <v>255758</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C6">
-        <v>5.867236584612215</v>
+        <v>24.41543356107163</v>
       </c>
       <c r="D6">
-        <v>83.40736760144556</v>
+        <v>88.65038914295393</v>
       </c>
       <c r="E6">
-        <v>0.03891326946682842</v>
+        <v>0.04454611910051697</v>
       </c>
       <c r="F6">
-        <v>0.282</v>
+        <v>0.255</v>
       </c>
       <c r="G6">
-        <v>0.897</v>
+        <v>0.288</v>
       </c>
       <c r="H6" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="I6">
-        <v>0.72</v>
+        <v>0.82</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="L6" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
-        <v>53163</v>
+        <v>32155</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C7">
-        <v>5.867236584612215</v>
+        <v>3.943889403874984</v>
       </c>
       <c r="D7">
-        <v>83.40736760144556</v>
+        <v>122.2375815137479</v>
       </c>
       <c r="E7">
-        <v>0.03891326946682842</v>
+        <v>0.06142341750908555</v>
       </c>
       <c r="F7">
-        <v>0.321</v>
+        <v>0.316</v>
       </c>
       <c r="G7">
-        <v>0.792</v>
+        <v>0.361</v>
       </c>
       <c r="H7" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="I7">
-        <v>0.72</v>
+        <v>0.82</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="L7" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>218680</v>
+        <v>228763</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C8">
-        <v>21.02082832652407</v>
+        <v>21.9439580686877</v>
       </c>
       <c r="D8">
-        <v>36.25037373747465</v>
+        <v>48.218553659693</v>
       </c>
       <c r="E8">
-        <v>0.01691242155321472</v>
+        <v>0.02422944168598808</v>
       </c>
       <c r="F8">
-        <v>0.338</v>
+        <v>0.34</v>
       </c>
       <c r="G8">
-        <v>0.901</v>
+        <v>0.535</v>
       </c>
       <c r="H8" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="I8">
-        <v>0.34</v>
+        <v>0.28</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K8" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="L8" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>2472</v>
+        <v>10646</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9">
-        <v>1.22631922271432</v>
+        <v>1.974674128242982</v>
       </c>
       <c r="D9">
-        <v>189.714282154569</v>
+        <v>169.6591140654627</v>
       </c>
       <c r="E9">
-        <v>0.08851020234163003</v>
+        <v>0.08525236239472268</v>
       </c>
       <c r="F9">
         <v>0.426</v>
       </c>
       <c r="G9">
-        <v>0.273</v>
+        <v>0.034</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="I9">
-        <v>0.34</v>
+        <v>0.28</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K9" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="L9" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>218680</v>
+        <v>87317</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C10">
-        <v>21.02082832652407</v>
+        <v>8.994140602648173</v>
       </c>
       <c r="D10">
-        <v>36.25037373747465</v>
+        <v>36.07034710075925</v>
       </c>
       <c r="E10">
-        <v>0.01691242155321472</v>
+        <v>0.0181250640124812</v>
       </c>
       <c r="F10">
-        <v>0.443</v>
+        <v>0.444</v>
       </c>
       <c r="G10">
-        <v>0.481</v>
+        <v>0.478</v>
       </c>
       <c r="H10" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="I10">
-        <v>0.08</v>
+        <v>0.41</v>
       </c>
       <c r="J10">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K10" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="L10" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11">
-        <v>14663</v>
+        <v>10646</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C11">
-        <v>2.342442865153752</v>
+        <v>1.974674128242982</v>
       </c>
       <c r="D11">
-        <v>160.2137526218972</v>
+        <v>169.6591140654627</v>
       </c>
       <c r="E11">
-        <v>0.07474688516556925</v>
+        <v>0.08525236239472268</v>
       </c>
       <c r="F11">
-        <v>0.518</v>
+        <v>0.529</v>
       </c>
       <c r="G11">
-        <v>0.511</v>
+        <v>0.52</v>
       </c>
       <c r="H11" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="I11">
-        <v>0.08</v>
+        <v>0.41</v>
       </c>
       <c r="J11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K11" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L11" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12">
-        <v>53163</v>
+        <v>12963</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="C12">
-        <v>5.867236584612215</v>
+        <v>2.186802622995846</v>
       </c>
       <c r="D12">
-        <v>83.40736760144556</v>
+        <v>164.1780270220661</v>
       </c>
       <c r="E12">
-        <v>0.03891326946682842</v>
+        <v>0.08249815952436955</v>
       </c>
       <c r="F12">
-        <v>0.5570000000000001</v>
+        <v>0.611</v>
       </c>
       <c r="G12">
-        <v>0.575</v>
+        <v>0.902</v>
       </c>
       <c r="H12" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="I12">
-        <v>0.34</v>
+        <v>0.99</v>
       </c>
       <c r="J12">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="L12" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13">
-        <v>53163</v>
+        <v>63122</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="C13">
-        <v>5.867236584612215</v>
+        <v>6.779013744406678</v>
       </c>
       <c r="D13">
-        <v>83.40736760144556</v>
+        <v>67.58461501465429</v>
       </c>
       <c r="E13">
-        <v>0.03891326946682842</v>
+        <v>0.03396073428341704</v>
       </c>
       <c r="F13">
-        <v>0.596</v>
+        <v>0.645</v>
       </c>
       <c r="G13">
-        <v>0.258</v>
+        <v>0.924</v>
       </c>
       <c r="H13" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="I13">
-        <v>0.34</v>
+        <v>0.99</v>
       </c>
       <c r="J13">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="L13" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14">
-        <v>31096</v>
+        <v>105749</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C14">
-        <v>3.846934688318971</v>
+        <v>10.68164703997437</v>
       </c>
       <c r="D14">
-        <v>124.3908658466227</v>
+        <v>18.64817228736216</v>
       </c>
       <c r="E14">
-        <v>0.05803390541026786</v>
+        <v>0.009370559021238324</v>
       </c>
       <c r="F14">
-        <v>0.654</v>
+        <v>0.655</v>
       </c>
       <c r="G14">
-        <v>0.522</v>
+        <v>0.388</v>
       </c>
       <c r="H14" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I14">
-        <v>0.85</v>
+        <v>0.23</v>
       </c>
       <c r="J14">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K14" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15">
-        <v>218631</v>
+        <v>87304</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C15">
-        <v>21.01634222542658</v>
+        <v>8.992950412561083</v>
       </c>
       <c r="D15">
-        <v>36.19637377345086</v>
+        <v>36.08464474595007</v>
       </c>
       <c r="E15">
-        <v>0.01688722815349855</v>
+        <v>0.01813224846605985</v>
       </c>
       <c r="F15">
-        <v>0.671</v>
+        <v>0.673</v>
       </c>
       <c r="G15">
-        <v>0.727</v>
+        <v>0.491</v>
       </c>
       <c r="H15" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="I15">
-        <v>0.85</v>
+        <v>0.23</v>
       </c>
       <c r="J15">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K15" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="L15" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16">
-        <v>30912</v>
+        <v>81302</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="C16">
-        <v>3.830088920932468</v>
+        <v>8.443448804660051</v>
       </c>
       <c r="D16">
-        <v>124.7669135142756</v>
+        <v>42.98836357711372</v>
       </c>
       <c r="E16">
-        <v>0.05820934847536583</v>
+        <v>0.02160131255323021</v>
       </c>
       <c r="F16">
-        <v>0.729</v>
+        <v>0.695</v>
       </c>
       <c r="G16">
-        <v>0.8110000000000001</v>
+        <v>0.849</v>
       </c>
       <c r="H16" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I16">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
       <c r="J16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K16" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="L16" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17">
-        <v>60987</v>
+        <v>10720</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="C17">
-        <v>6.583547910873072</v>
+        <v>1.981449056431032</v>
       </c>
       <c r="D17">
-        <v>70.83666576856902</v>
+        <v>169.4826686703005</v>
       </c>
       <c r="E17">
-        <v>0.03304847452272566</v>
+        <v>0.08516369997977308</v>
       </c>
       <c r="F17">
-        <v>0.762</v>
+        <v>0.78</v>
       </c>
       <c r="G17">
-        <v>0.699</v>
+        <v>0.291</v>
       </c>
       <c r="H17" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="I17">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
       <c r="J17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K17" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="L17" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18">
-        <v>2491</v>
+        <v>58645</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C18">
-        <v>1.228058731303144</v>
+        <v>6.369130589029652</v>
       </c>
       <c r="D18">
-        <v>189.6663663084356</v>
+        <v>74.49190678922365</v>
       </c>
       <c r="E18">
-        <v>0.08848784745517405</v>
+        <v>0.03743159374637794</v>
       </c>
       <c r="F18">
-        <v>0.851</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="G18">
-        <v>0.952</v>
+        <v>0.63</v>
       </c>
       <c r="H18" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="I18">
-        <v>0.5600000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="J18">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K18" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19">
-        <v>60968</v>
+        <v>87822</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C19">
-        <v>6.581808402284249</v>
+        <v>9.040374909877432</v>
       </c>
       <c r="D19">
-        <v>70.86594977585207</v>
+        <v>35.51713121481843</v>
       </c>
       <c r="E19">
-        <v>0.03306213682258289</v>
+        <v>0.01784707740710174</v>
       </c>
       <c r="F19">
-        <v>0.884</v>
+        <v>0.835</v>
       </c>
       <c r="G19">
-        <v>0.619</v>
+        <v>0.326</v>
       </c>
       <c r="H19" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="I19">
-        <v>0.5600000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="J19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K19" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="L19" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20">
-        <v>30912</v>
+        <v>12949</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="C20">
-        <v>3.830088920932468</v>
+        <v>2.185520879825134</v>
       </c>
       <c r="D20">
-        <v>124.7669135142756</v>
+        <v>164.2108751213976</v>
       </c>
       <c r="E20">
-        <v>0.05820934847536583</v>
+        <v>0.08251466543437391</v>
       </c>
       <c r="F20">
-        <v>0.9419999999999999</v>
+        <v>0.917</v>
       </c>
       <c r="G20">
-        <v>0.157</v>
+        <v>0.051</v>
       </c>
       <c r="H20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I20">
-        <v>0.41</v>
+        <v>0.57</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="K20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21">
-        <v>30912</v>
+        <v>12946</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="C21">
-        <v>3.830088920932468</v>
+        <v>2.185246220574267</v>
       </c>
       <c r="D21">
-        <v>124.7669135142756</v>
+        <v>164.2179144273061</v>
       </c>
       <c r="E21">
-        <v>0.05820934847536583</v>
+        <v>0.08251820262989461</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21">
-        <v>0.859</v>
+        <v>0.91</v>
       </c>
       <c r="H21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I21">
-        <v>0.41</v>
+        <v>0.57</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="K21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated func for report
</commit_message>
<xml_diff>
--- a/GA.xlsx
+++ b/GA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual Code\IA_AlgoritmoGenetico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFBA71D-3494-47AC-99E9-67D80DB37CE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82E51C7-5668-4856-B3D0-69D345404679}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GER 1" sheetId="1" r:id="rId1"/>
@@ -246,6 +246,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -275,9 +278,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1491,6 +1495,18 @@
         <v>50</v>
       </c>
     </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <f>AVERAGE(D2:D21)</f>
+        <v>42.292169999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <f>LARGE(D2:D21,1)</f>
+        <v>181.92339999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1498,9 +1514,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1564,7 +1582,7 @@
       <c r="E2">
         <v>8.6499999999999994E-2</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>8.6499999999999994E-2</v>
       </c>
       <c r="G2">
@@ -1605,7 +1623,7 @@
       <c r="E3">
         <v>4.6100000000000002E-2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>0.1326</v>
       </c>
       <c r="G3">
@@ -1646,7 +1664,7 @@
       <c r="E4">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>0.1542</v>
       </c>
       <c r="G4">
@@ -1687,7 +1705,7 @@
       <c r="E5">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>0.1633</v>
       </c>
       <c r="G5">
@@ -1728,7 +1746,7 @@
       <c r="E6">
         <v>2.9600000000000001E-2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>0.19289999999999999</v>
       </c>
       <c r="G6">
@@ -1769,7 +1787,7 @@
       <c r="E7">
         <v>8.6699999999999999E-2</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>0.27960000000000002</v>
       </c>
       <c r="G7">
@@ -1810,7 +1828,7 @@
       <c r="E8">
         <v>4.0099999999999997E-2</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>0.31969999999999998</v>
       </c>
       <c r="G8">
@@ -1851,7 +1869,7 @@
       <c r="E9">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>0.34129999999999999</v>
       </c>
       <c r="G9">
@@ -1892,7 +1910,7 @@
       <c r="E10">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>0.3629</v>
       </c>
       <c r="G10">
@@ -1933,7 +1951,7 @@
       <c r="E11">
         <v>3.4200000000000001E-2</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>0.39710000000000001</v>
       </c>
       <c r="G11">
@@ -1974,7 +1992,7 @@
       <c r="E12">
         <v>8.6499999999999994E-2</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>0.48359999999999997</v>
       </c>
       <c r="G12">
@@ -2015,7 +2033,7 @@
       <c r="E13">
         <v>8.6499999999999994E-2</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>0.57010000000000005</v>
       </c>
       <c r="G13">
@@ -2056,7 +2074,7 @@
       <c r="E14">
         <v>4.5100000000000001E-2</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>0.61519999999999997</v>
       </c>
       <c r="G14">
@@ -2097,7 +2115,7 @@
       <c r="E15">
         <v>8.72E-2</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>0.70240000000000002</v>
       </c>
       <c r="G15">
@@ -2138,7 +2156,7 @@
       <c r="E16">
         <v>8.6499999999999994E-2</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>0.78890000000000005</v>
       </c>
       <c r="G16">
@@ -2179,7 +2197,7 @@
       <c r="E17">
         <v>8.6499999999999994E-2</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>0.87539999999999996</v>
       </c>
       <c r="G17">
@@ -2220,7 +2238,7 @@
       <c r="E18">
         <v>4.5600000000000002E-2</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>0.92100000000000004</v>
       </c>
       <c r="G18">
@@ -2261,7 +2279,7 @@
       <c r="E19">
         <v>4.7000000000000002E-3</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>0.92569999999999997</v>
       </c>
       <c r="G19">
@@ -2302,7 +2320,7 @@
       <c r="E20">
         <v>3.4099999999999998E-2</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>0.95979999999999999</v>
       </c>
       <c r="G20">
@@ -2343,7 +2361,7 @@
       <c r="E21">
         <v>4.0099999999999997E-2</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>0.99990000000000001</v>
       </c>
       <c r="G21">
@@ -2366,6 +2384,18 @@
       </c>
       <c r="M21" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <f>AVERAGE(D2:D21)</f>
+        <v>105.13188499999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <f>LARGE(D2:D21,1)</f>
+        <v>183.42099999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2375,9 +2405,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3245,6 +3277,12 @@
         <v>20</v>
       </c>
     </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <f>AVERAGE(D2:D21)</f>
+        <v>155.69884000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>